<commit_message>
Added Updates & Walkthrough video
</commit_message>
<xml_diff>
--- a/EgyBestSeriesBot/Data/Config.xlsx
+++ b/EgyBestSeriesBot/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MyProjects\UiPath\EgyBestSeriesBot\EgyBestSeriesBot\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\RPA\UiPath\EgyBestSeriesBot\EgyBestSeriesBot\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CC81EC4-8E6E-4DF4-95EF-65D1D4122672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA82812-357C-4B16-B5DA-CCAA51D2F9FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11280" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
   <si>
     <t>Name</t>
   </si>
@@ -127,9 +127,6 @@
   </si>
   <si>
     <t>VidStreamDownloadBtnClass</t>
-  </si>
-  <si>
-    <t>VidStreamDownloadBtnPostDelay</t>
   </si>
   <si>
     <t>The path of the folder which will contain the downloadable links</t>
@@ -655,7 +652,7 @@
         <v>23</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
@@ -667,7 +664,7 @@
         <v>21</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1669,10 +1666,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z997"/>
+  <dimension ref="A1:Z996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1777,124 +1774,117 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A11" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11" s="5">
-        <v>3000</v>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="5">
+        <v>500</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" s="5" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B13" s="5">
-        <v>500</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" s="5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B14" s="5">
-        <v>2000</v>
+        <v>15000</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B15" s="5">
-        <v>15000</v>
+        <v>60000</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A16" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="5">
-        <v>60000</v>
+    <row r="17" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="5">
+        <v>3</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="14.25" customHeight="1">
+    <row r="18" spans="1:3">
       <c r="A18" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" s="5">
-        <v>3</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>36</v>
+        <v>10</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="B19" s="9"/>
+      <c r="C19" s="7"/>
     </row>
-    <row r="20" spans="1:3">
-      <c r="B20" s="9"/>
-      <c r="C20" s="7"/>
+    <row r="20" spans="1:3" ht="105">
+      <c r="A20" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="12"/>
     </row>
-    <row r="21" spans="1:3" ht="105">
-      <c r="A21" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B21" s="14" t="s">
-        <v>16</v>
-      </c>
+    <row r="21" spans="1:3">
+      <c r="A21" s="13"/>
+      <c r="B21" s="13"/>
       <c r="C21" s="12"/>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="13"/>
-      <c r="B22" s="13"/>
+      <c r="A22" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>18</v>
+      </c>
       <c r="C22" s="12"/>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="13" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C23" s="12"/>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>20</v>
-      </c>
+      <c r="A24" s="13"/>
+      <c r="B24" s="13"/>
       <c r="C24" s="12"/>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="13"/>
-      <c r="B25" s="13"/>
-      <c r="C25" s="12"/>
+      <c r="A25" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="7"/>
     </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C26" s="7"/>
-    </row>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
     <row r="36" ht="14.25" customHeight="1"/>
     <row r="37" ht="14.25" customHeight="1"/>
@@ -2857,7 +2847,6 @@
     <row r="994" ht="14.25" customHeight="1"/>
     <row r="995" ht="14.25" customHeight="1"/>
     <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Handling invalid characters in series name
</commit_message>
<xml_diff>
--- a/EgyBestSeriesBot/Data/Config.xlsx
+++ b/EgyBestSeriesBot/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\RPA\UiPath\EgyBestSeriesBot\EgyBestSeriesBot\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MyProjects\UiPath\EgyBestSeriesBot\EgyBestSeriesBot\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA82812-357C-4B16-B5DA-CCAA51D2F9FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C4C321-7E9B-4CFB-93EF-4EA4F74AE172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11280" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1668,8 +1668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z996"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
Handling pop-up ads blocker
</commit_message>
<xml_diff>
--- a/EgyBestSeriesBot/Data/Config.xlsx
+++ b/EgyBestSeriesBot/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MyProjects\UiPath\EgyBestSeriesBot\EgyBestSeriesBot\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\RPA\UiPath\EgyBestSeriesBot\EgyBestSeriesBot\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C4C321-7E9B-4CFB-93EF-4EA4F74AE172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8DB4863-E2D1-49F2-B573-444C28D96D77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11280" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
   <si>
     <t>Name</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t>Exceptions Screenshots</t>
+  </si>
+  <si>
+    <t>PopUpAdsBlockerDelay</t>
   </si>
 </sst>
 </file>
@@ -1666,10 +1669,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z996"/>
+  <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1807,85 +1810,92 @@
         <v>60000</v>
       </c>
     </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="5">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A19" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B19" s="5">
         <v>3</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C19" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="5" t="s">
+    <row r="20" spans="1:3">
+      <c r="A20" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B20" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C20" s="6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="B19" s="9"/>
-      <c r="C19" s="7"/>
-    </row>
-    <row r="20" spans="1:3" ht="105">
-      <c r="A20" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" s="12"/>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="13"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="12"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="7"/>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" ht="105">
       <c r="A22" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B22" s="13" t="s">
-        <v>18</v>
+        <v>15</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>16</v>
       </c>
       <c r="C22" s="12"/>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>20</v>
-      </c>
+      <c r="A23" s="13"/>
+      <c r="B23" s="13"/>
       <c r="C23" s="12"/>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="13"/>
-      <c r="B24" s="13"/>
+      <c r="A24" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>18</v>
+      </c>
       <c r="C24" s="12"/>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" s="12"/>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="13"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="12"/>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B27" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C25" s="7"/>
+      <c r="C27" s="7"/>
     </row>
-    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="36" ht="14.25" customHeight="1"/>
     <row r="37" ht="14.25" customHeight="1"/>
     <row r="38" ht="14.25" customHeight="1"/>
@@ -2847,6 +2857,8 @@
     <row r="994" ht="14.25" customHeight="1"/>
     <row r="995" ht="14.25" customHeight="1"/>
     <row r="996" ht="14.25" customHeight="1"/>
+    <row r="997" ht="14.25" customHeight="1"/>
+    <row r="998" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>